<commit_message>
Updates to asset swap pricing, Added InflationLinkedSwap, Added Lagged CPI formulae
</commit_message>
<xml_diff>
--- a/ExcelExamples/ZARAssetSwap.xlsx
+++ b/ExcelExamples/ZARAssetSwap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ines Moussi\Source\Repos\QuantSA\QuantSA\QuantSA.Excel.AddIn\bin\Debug\ExcelExamples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ines Moussi\Source\Repos\QuantSA\ExcelExamples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1E9EDF-161D-499B-A136-57069190B001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1EF3802-8722-4B19-B244-CEF7539CA755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{22AAC177-9997-449C-8BA1-AEA9B7E68A8A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{22AAC177-9997-449C-8BA1-AEA9B7E68A8A}"/>
   </bookViews>
   <sheets>
     <sheet name="createUnderlyingBesaJSEBond" sheetId="2" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>name</t>
   </si>
@@ -1977,8 +1977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8BB9563-6356-4D0C-AAB3-63DD00989230}">
   <dimension ref="B2:H98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2068,6 +2068,9 @@
       <c r="E7" s="5">
         <v>41391</v>
       </c>
+      <c r="G7" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="H7" s="2" t="str" cm="1">
         <f t="array" ref="H7">_xll.QSA.CreateAssetSwap(C2,C4,createUnderlyingBesaJSEBond!B14,createAssetSwap!C5,C7,C6,E3:E98,C3,H3)</f>
         <v>assetSwap.11:31:51-4</v>
@@ -2730,8 +2733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA128FE-9F47-40CB-A7B8-579CE50E3113}">
   <dimension ref="B2:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>